<commit_message>
refactored probs and preparation
</commit_message>
<xml_diff>
--- a/data/processed/poblacion.xlsx
+++ b/data/processed/poblacion.xlsx
@@ -74,7 +74,7 @@
     <t xml:space="preserve">Pensión</t>
   </si>
   <si>
-    <t xml:space="preserve">F</t>
+    <t xml:space="preserve">f</t>
   </si>
   <si>
     <t xml:space="preserve">ASECONTRALORIA</t>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">RENUNCIA</t>
   </si>
   <si>
-    <t xml:space="preserve">M</t>
+    <t xml:space="preserve">m</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>

</xml_diff>